<commit_message>
fixed typos in the description
</commit_message>
<xml_diff>
--- a/ACQ.Excel/Examples/ACQ.Options.xlsx
+++ b/ACQ.Excel/Examples/ACQ.Options.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\ACQ\ACQ.Excel\Examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F672C4AA-D820-4D13-98EB-7BD17E8327C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B0010A3-C0B0-48A6-835C-6F4DAD829E24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Utils" sheetId="3" r:id="rId1"/>
@@ -829,7 +829,7 @@
     <numFmt numFmtId="167" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
     <numFmt numFmtId="168" formatCode="0.0%"/>
     <numFmt numFmtId="169" formatCode="0.0000000000000000000000000E+00"/>
-    <numFmt numFmtId="173" formatCode="0.0"/>
+    <numFmt numFmtId="170" formatCode="0.0"/>
   </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
@@ -1302,14 +1302,14 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="20" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="21" xfId="2" applyBorder="1"/>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="2" applyFont="1"/>
+    <xf numFmtId="170" fontId="3" fillId="3" borderId="2" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="3" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="18" xfId="8" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="2" applyFont="1"/>
-    <xf numFmtId="173" fontId="3" fillId="3" borderId="2" xfId="2" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="20% - Accent3" xfId="7" builtinId="38"/>
@@ -15977,8 +15977,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B2:N56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27090,8 +27090,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57EC0629-1DDD-4850-A456-ABCD64977042}">
   <dimension ref="B1:AK45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V2" sqref="V2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27418,7 +27418,7 @@
       <c r="AA6" t="s">
         <v>181</v>
       </c>
-      <c r="AB6" s="59">
+      <c r="AB6" s="57">
         <v>0</v>
       </c>
       <c r="AD6">
@@ -28808,7 +28808,7 @@
       <c r="B25" t="s">
         <v>181</v>
       </c>
-      <c r="C25" s="60">
+      <c r="C25" s="58">
         <v>0</v>
       </c>
       <c r="F25">
@@ -30178,37 +30178,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="60" t="s">
         <v>129</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
     </row>
     <row r="2" spans="1:43" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F2" s="57" t="s">
+      <c r="F2" s="59" t="s">
         <v>97</v>
       </c>
-      <c r="G2" s="57"/>
-      <c r="H2" s="57"/>
-      <c r="I2" s="57"/>
-      <c r="L2" s="57" t="s">
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="59"/>
+      <c r="L2" s="59" t="s">
         <v>98</v>
       </c>
-      <c r="M2" s="57"/>
-      <c r="N2" s="57"/>
-      <c r="O2" s="57"/>
-      <c r="P2" s="57"/>
-      <c r="S2" s="57" t="s">
+      <c r="M2" s="59"/>
+      <c r="N2" s="59"/>
+      <c r="O2" s="59"/>
+      <c r="P2" s="59"/>
+      <c r="S2" s="59" t="s">
         <v>107</v>
       </c>
-      <c r="T2" s="57"/>
-      <c r="U2" s="57"/>
-      <c r="V2" s="57"/>
-      <c r="W2" s="57"/>
-      <c r="X2" s="57"/>
-      <c r="Y2" s="57"/>
-      <c r="Z2" s="57"/>
+      <c r="T2" s="59"/>
+      <c r="U2" s="59"/>
+      <c r="V2" s="59"/>
+      <c r="W2" s="59"/>
+      <c r="X2" s="59"/>
+      <c r="Y2" s="59"/>
+      <c r="Z2" s="59"/>
       <c r="AB2" s="3" t="s">
         <v>112</v>
       </c>
@@ -31383,16 +31383,16 @@
         <f>_xll.acq_options_black_vol($C$4,$C$5,$C$6,$C$8,N17,FALSE)</f>
         <v>0.65000000000000013</v>
       </c>
-      <c r="S17" s="57" t="s">
+      <c r="S17" s="59" t="s">
         <v>108</v>
       </c>
-      <c r="T17" s="57"/>
-      <c r="U17" s="57"/>
-      <c r="V17" s="57"/>
-      <c r="W17" s="57"/>
-      <c r="X17" s="57"/>
-      <c r="Y17" s="57"/>
-      <c r="Z17" s="57"/>
+      <c r="T17" s="59"/>
+      <c r="U17" s="59"/>
+      <c r="V17" s="59"/>
+      <c r="W17" s="59"/>
+      <c r="X17" s="59"/>
+      <c r="Y17" s="59"/>
+      <c r="Z17" s="59"/>
       <c r="AB17" s="16">
         <f>C7</f>
         <v>0.2</v>
@@ -32573,37 +32573,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="60" t="s">
         <v>128</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
     </row>
     <row r="2" spans="1:43" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F2" s="57" t="s">
+      <c r="F2" s="59" t="s">
         <v>97</v>
       </c>
-      <c r="G2" s="57"/>
-      <c r="H2" s="57"/>
-      <c r="I2" s="57"/>
-      <c r="L2" s="57" t="s">
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="59"/>
+      <c r="L2" s="59" t="s">
         <v>98</v>
       </c>
-      <c r="M2" s="57"/>
-      <c r="N2" s="57"/>
-      <c r="O2" s="57"/>
-      <c r="P2" s="57"/>
-      <c r="S2" s="57" t="s">
+      <c r="M2" s="59"/>
+      <c r="N2" s="59"/>
+      <c r="O2" s="59"/>
+      <c r="P2" s="59"/>
+      <c r="S2" s="59" t="s">
         <v>107</v>
       </c>
-      <c r="T2" s="57"/>
-      <c r="U2" s="57"/>
-      <c r="V2" s="57"/>
-      <c r="W2" s="57"/>
-      <c r="X2" s="57"/>
-      <c r="Y2" s="57"/>
-      <c r="Z2" s="57"/>
+      <c r="T2" s="59"/>
+      <c r="U2" s="59"/>
+      <c r="V2" s="59"/>
+      <c r="W2" s="59"/>
+      <c r="X2" s="59"/>
+      <c r="Y2" s="59"/>
+      <c r="Z2" s="59"/>
       <c r="AB2" s="3" t="s">
         <v>112</v>
       </c>
@@ -33778,16 +33778,16 @@
         <f>_xll.acq_options_bachelier_vol($C$4,$C$5,$C$6,$C$8,N17,FALSE)</f>
         <v>25.999999999962554</v>
       </c>
-      <c r="S17" s="57" t="s">
+      <c r="S17" s="59" t="s">
         <v>108</v>
       </c>
-      <c r="T17" s="57"/>
-      <c r="U17" s="57"/>
-      <c r="V17" s="57"/>
-      <c r="W17" s="57"/>
-      <c r="X17" s="57"/>
-      <c r="Y17" s="57"/>
-      <c r="Z17" s="57"/>
+      <c r="T17" s="59"/>
+      <c r="U17" s="59"/>
+      <c r="V17" s="59"/>
+      <c r="W17" s="59"/>
+      <c r="X17" s="59"/>
+      <c r="Y17" s="59"/>
+      <c r="Z17" s="59"/>
       <c r="AB17" s="16">
         <f>C7</f>
         <v>20</v>
@@ -34664,14 +34664,14 @@
       </c>
     </row>
     <row r="32" spans="6:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L32" s="57" t="s">
+      <c r="L32" s="59" t="s">
         <v>131</v>
       </c>
-      <c r="M32" s="57"/>
-      <c r="N32" s="57"/>
-      <c r="O32" s="57"/>
-      <c r="P32" s="57"/>
-      <c r="Q32" s="57"/>
+      <c r="M32" s="59"/>
+      <c r="N32" s="59"/>
+      <c r="O32" s="59"/>
+      <c r="P32" s="59"/>
+      <c r="Q32" s="59"/>
       <c r="AB32" t="s">
         <v>111</v>
       </c>
@@ -35331,37 +35331,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:45" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="60" t="s">
         <v>130</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
     </row>
     <row r="2" spans="1:45" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F2" s="57" t="s">
+      <c r="F2" s="59" t="s">
         <v>97</v>
       </c>
-      <c r="G2" s="57"/>
-      <c r="H2" s="57"/>
-      <c r="I2" s="57"/>
-      <c r="L2" s="57" t="s">
+      <c r="G2" s="59"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="59"/>
+      <c r="L2" s="59" t="s">
         <v>98</v>
       </c>
-      <c r="M2" s="57"/>
-      <c r="N2" s="57"/>
-      <c r="O2" s="57"/>
-      <c r="P2" s="57"/>
-      <c r="S2" s="57" t="s">
+      <c r="M2" s="59"/>
+      <c r="N2" s="59"/>
+      <c r="O2" s="59"/>
+      <c r="P2" s="59"/>
+      <c r="S2" s="59" t="s">
         <v>107</v>
       </c>
-      <c r="T2" s="57"/>
-      <c r="U2" s="57"/>
-      <c r="V2" s="57"/>
-      <c r="W2" s="57"/>
-      <c r="X2" s="57"/>
-      <c r="Y2" s="57"/>
-      <c r="Z2" s="57"/>
+      <c r="T2" s="59"/>
+      <c r="U2" s="59"/>
+      <c r="V2" s="59"/>
+      <c r="W2" s="59"/>
+      <c r="X2" s="59"/>
+      <c r="Y2" s="59"/>
+      <c r="Z2" s="59"/>
       <c r="AA2" s="37"/>
       <c r="AB2" s="37"/>
       <c r="AD2" s="3" t="s">
@@ -36638,16 +36638,16 @@
         <f>_xll.acq_options_blackscholes_vol($C$4,$C$5,$C$6,$C$8,$C$9,$N17,FALSE)</f>
         <v>0.65</v>
       </c>
-      <c r="S17" s="57" t="s">
+      <c r="S17" s="59" t="s">
         <v>108</v>
       </c>
-      <c r="T17" s="57"/>
-      <c r="U17" s="57"/>
-      <c r="V17" s="57"/>
-      <c r="W17" s="57"/>
-      <c r="X17" s="57"/>
-      <c r="Y17" s="57"/>
-      <c r="Z17" s="57"/>
+      <c r="T17" s="59"/>
+      <c r="U17" s="59"/>
+      <c r="V17" s="59"/>
+      <c r="W17" s="59"/>
+      <c r="X17" s="59"/>
+      <c r="Y17" s="59"/>
+      <c r="Z17" s="59"/>
       <c r="AA17" s="37"/>
       <c r="AB17" s="37"/>
       <c r="AD17" s="16">
@@ -38271,15 +38271,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="60" t="s">
         <v>135</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
     </row>
     <row r="2" spans="1:28" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="L2" t="s">
@@ -38294,15 +38294,15 @@
         <v>92</v>
       </c>
       <c r="C3" s="3"/>
-      <c r="F3" s="57" t="s">
+      <c r="F3" s="59" t="s">
         <v>139</v>
       </c>
-      <c r="G3" s="57"/>
-      <c r="H3" s="57"/>
-      <c r="I3" s="57" t="s">
+      <c r="G3" s="59"/>
+      <c r="H3" s="59"/>
+      <c r="I3" s="59" t="s">
         <v>137</v>
       </c>
-      <c r="J3" s="57"/>
+      <c r="J3" s="59"/>
       <c r="M3" t="s">
         <v>144</v>
       </c>
@@ -40061,26 +40061,26 @@
       <c r="Z29" s="46"/>
     </row>
     <row r="30" spans="6:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G30" s="57" t="s">
+      <c r="G30" s="59" t="s">
         <v>145</v>
       </c>
-      <c r="H30" s="57"/>
-      <c r="I30" s="57"/>
-      <c r="J30" s="57"/>
-      <c r="K30" s="57"/>
-      <c r="L30" s="57"/>
-      <c r="M30" s="57"/>
-      <c r="N30" s="57"/>
-      <c r="S30" s="57" t="s">
+      <c r="H30" s="59"/>
+      <c r="I30" s="59"/>
+      <c r="J30" s="59"/>
+      <c r="K30" s="59"/>
+      <c r="L30" s="59"/>
+      <c r="M30" s="59"/>
+      <c r="N30" s="59"/>
+      <c r="S30" s="59" t="s">
         <v>146</v>
       </c>
-      <c r="T30" s="57"/>
-      <c r="U30" s="57"/>
-      <c r="V30" s="57"/>
-      <c r="W30" s="57"/>
-      <c r="X30" s="57"/>
-      <c r="Y30" s="57"/>
-      <c r="Z30" s="57"/>
+      <c r="T30" s="59"/>
+      <c r="U30" s="59"/>
+      <c r="V30" s="59"/>
+      <c r="W30" s="59"/>
+      <c r="X30" s="59"/>
+      <c r="Y30" s="59"/>
+      <c r="Z30" s="59"/>
     </row>
     <row r="31" spans="6:28" x14ac:dyDescent="0.25">
       <c r="F31" t="s">
@@ -40949,26 +40949,26 @@
       <c r="AB44" s="46"/>
     </row>
     <row r="45" spans="6:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G45" s="57" t="s">
+      <c r="G45" s="59" t="s">
         <v>148</v>
       </c>
-      <c r="H45" s="57"/>
-      <c r="I45" s="57"/>
-      <c r="J45" s="57"/>
-      <c r="K45" s="57"/>
-      <c r="L45" s="57"/>
-      <c r="M45" s="57"/>
-      <c r="N45" s="57"/>
-      <c r="S45" s="57" t="s">
+      <c r="H45" s="59"/>
+      <c r="I45" s="59"/>
+      <c r="J45" s="59"/>
+      <c r="K45" s="59"/>
+      <c r="L45" s="59"/>
+      <c r="M45" s="59"/>
+      <c r="N45" s="59"/>
+      <c r="S45" s="59" t="s">
         <v>147</v>
       </c>
-      <c r="T45" s="57"/>
-      <c r="U45" s="57"/>
-      <c r="V45" s="57"/>
-      <c r="W45" s="57"/>
-      <c r="X45" s="57"/>
-      <c r="Y45" s="57"/>
-      <c r="Z45" s="57"/>
+      <c r="T45" s="59"/>
+      <c r="U45" s="59"/>
+      <c r="V45" s="59"/>
+      <c r="W45" s="59"/>
+      <c r="X45" s="59"/>
+      <c r="Y45" s="59"/>
+      <c r="Z45" s="59"/>
       <c r="AA45" s="46"/>
       <c r="AB45" s="46"/>
     </row>
@@ -41857,15 +41857,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:46" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="60" t="s">
         <v>162</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
     </row>
     <row r="2" spans="1:46" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="L2" t="s">
@@ -41886,15 +41886,15 @@
         <v>92</v>
       </c>
       <c r="C3" s="3"/>
-      <c r="F3" s="57" t="s">
+      <c r="F3" s="59" t="s">
         <v>139</v>
       </c>
-      <c r="G3" s="57"/>
-      <c r="H3" s="57"/>
-      <c r="I3" s="57" t="s">
+      <c r="G3" s="59"/>
+      <c r="H3" s="59"/>
+      <c r="I3" s="59" t="s">
         <v>163</v>
       </c>
-      <c r="J3" s="57"/>
+      <c r="J3" s="59"/>
       <c r="M3" t="s">
         <v>144</v>
       </c>
@@ -44889,26 +44889,26 @@
       </c>
     </row>
     <row r="30" spans="6:46" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G30" s="57" t="s">
+      <c r="G30" s="59" t="s">
         <v>164</v>
       </c>
-      <c r="H30" s="57"/>
-      <c r="I30" s="57"/>
-      <c r="J30" s="57"/>
-      <c r="K30" s="57"/>
-      <c r="L30" s="57"/>
-      <c r="M30" s="57"/>
-      <c r="N30" s="57"/>
-      <c r="S30" s="57" t="s">
+      <c r="H30" s="59"/>
+      <c r="I30" s="59"/>
+      <c r="J30" s="59"/>
+      <c r="K30" s="59"/>
+      <c r="L30" s="59"/>
+      <c r="M30" s="59"/>
+      <c r="N30" s="59"/>
+      <c r="S30" s="59" t="s">
         <v>167</v>
       </c>
-      <c r="T30" s="57"/>
-      <c r="U30" s="57"/>
-      <c r="V30" s="57"/>
-      <c r="W30" s="57"/>
-      <c r="X30" s="57"/>
-      <c r="Y30" s="57"/>
-      <c r="Z30" s="57"/>
+      <c r="T30" s="59"/>
+      <c r="U30" s="59"/>
+      <c r="V30" s="59"/>
+      <c r="W30" s="59"/>
+      <c r="X30" s="59"/>
+      <c r="Y30" s="59"/>
+      <c r="Z30" s="59"/>
       <c r="AE30">
         <f t="shared" si="3"/>
         <v>0</v>
@@ -46617,26 +46617,26 @@
       </c>
     </row>
     <row r="45" spans="6:46" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G45" s="57" t="s">
+      <c r="G45" s="59" t="s">
         <v>165</v>
       </c>
-      <c r="H45" s="57"/>
-      <c r="I45" s="57"/>
-      <c r="J45" s="57"/>
-      <c r="K45" s="57"/>
-      <c r="L45" s="57"/>
-      <c r="M45" s="57"/>
-      <c r="N45" s="57"/>
-      <c r="S45" s="57" t="s">
+      <c r="H45" s="59"/>
+      <c r="I45" s="59"/>
+      <c r="J45" s="59"/>
+      <c r="K45" s="59"/>
+      <c r="L45" s="59"/>
+      <c r="M45" s="59"/>
+      <c r="N45" s="59"/>
+      <c r="S45" s="59" t="s">
         <v>166</v>
       </c>
-      <c r="T45" s="57"/>
-      <c r="U45" s="57"/>
-      <c r="V45" s="57"/>
-      <c r="W45" s="57"/>
-      <c r="X45" s="57"/>
-      <c r="Y45" s="57"/>
-      <c r="Z45" s="57"/>
+      <c r="T45" s="59"/>
+      <c r="U45" s="59"/>
+      <c r="V45" s="59"/>
+      <c r="W45" s="59"/>
+      <c r="X45" s="59"/>
+      <c r="Y45" s="59"/>
+      <c r="Z45" s="59"/>
       <c r="AA45" s="46"/>
       <c r="AB45" s="46"/>
       <c r="AE45">
@@ -47576,15 +47576,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="60" t="s">
         <v>162</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
     </row>
     <row r="2" spans="1:28" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="L2" t="s">
@@ -47599,15 +47599,15 @@
         <v>92</v>
       </c>
       <c r="C3" s="3"/>
-      <c r="F3" s="57" t="s">
+      <c r="F3" s="59" t="s">
         <v>171</v>
       </c>
-      <c r="G3" s="57"/>
-      <c r="H3" s="57"/>
-      <c r="I3" s="57" t="s">
+      <c r="G3" s="59"/>
+      <c r="H3" s="59"/>
+      <c r="I3" s="59" t="s">
         <v>163</v>
       </c>
-      <c r="J3" s="57"/>
+      <c r="J3" s="59"/>
       <c r="M3" t="s">
         <v>144</v>
       </c>
@@ -49380,26 +49380,26 @@
       <c r="Z29" s="46"/>
     </row>
     <row r="30" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G30" s="57" t="s">
+      <c r="G30" s="59" t="s">
         <v>172</v>
       </c>
-      <c r="H30" s="57"/>
-      <c r="I30" s="57"/>
-      <c r="J30" s="57"/>
-      <c r="K30" s="57"/>
-      <c r="L30" s="57"/>
-      <c r="M30" s="57"/>
-      <c r="N30" s="57"/>
-      <c r="S30" s="57" t="s">
+      <c r="H30" s="59"/>
+      <c r="I30" s="59"/>
+      <c r="J30" s="59"/>
+      <c r="K30" s="59"/>
+      <c r="L30" s="59"/>
+      <c r="M30" s="59"/>
+      <c r="N30" s="59"/>
+      <c r="S30" s="59" t="s">
         <v>167</v>
       </c>
-      <c r="T30" s="57"/>
-      <c r="U30" s="57"/>
-      <c r="V30" s="57"/>
-      <c r="W30" s="57"/>
-      <c r="X30" s="57"/>
-      <c r="Y30" s="57"/>
-      <c r="Z30" s="57"/>
+      <c r="T30" s="59"/>
+      <c r="U30" s="59"/>
+      <c r="V30" s="59"/>
+      <c r="W30" s="59"/>
+      <c r="X30" s="59"/>
+      <c r="Y30" s="59"/>
+      <c r="Z30" s="59"/>
     </row>
     <row r="31" spans="2:28" x14ac:dyDescent="0.25">
       <c r="F31" t="s">
@@ -50268,26 +50268,26 @@
       <c r="AB44" s="46"/>
     </row>
     <row r="45" spans="6:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G45" s="57" t="s">
+      <c r="G45" s="59" t="s">
         <v>173</v>
       </c>
-      <c r="H45" s="57"/>
-      <c r="I45" s="57"/>
-      <c r="J45" s="57"/>
-      <c r="K45" s="57"/>
-      <c r="L45" s="57"/>
-      <c r="M45" s="57"/>
-      <c r="N45" s="57"/>
-      <c r="S45" s="57" t="s">
+      <c r="H45" s="59"/>
+      <c r="I45" s="59"/>
+      <c r="J45" s="59"/>
+      <c r="K45" s="59"/>
+      <c r="L45" s="59"/>
+      <c r="M45" s="59"/>
+      <c r="N45" s="59"/>
+      <c r="S45" s="59" t="s">
         <v>166</v>
       </c>
-      <c r="T45" s="57"/>
-      <c r="U45" s="57"/>
-      <c r="V45" s="57"/>
-      <c r="W45" s="57"/>
-      <c r="X45" s="57"/>
-      <c r="Y45" s="57"/>
-      <c r="Z45" s="57"/>
+      <c r="T45" s="59"/>
+      <c r="U45" s="59"/>
+      <c r="V45" s="59"/>
+      <c r="W45" s="59"/>
+      <c r="X45" s="59"/>
+      <c r="Y45" s="59"/>
+      <c r="Z45" s="59"/>
       <c r="AA45" s="46"/>
       <c r="AB45" s="46"/>
     </row>
@@ -51175,15 +51175,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="60" t="s">
         <v>162</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
       <c r="I1">
         <f>_xll.acq_options_binomial_american_price($C$5,F14,$C$7,$C$9,$C$10,$C$8,FALSE,6)</f>
         <v>20.986795441796307</v>
@@ -51195,40 +51195,40 @@
         <v>170</v>
       </c>
       <c r="C3" s="3"/>
-      <c r="F3" s="57" t="s">
+      <c r="F3" s="59" t="s">
         <v>139</v>
       </c>
-      <c r="G3" s="57"/>
-      <c r="H3" s="57"/>
-      <c r="I3" s="57" t="s">
+      <c r="G3" s="59"/>
+      <c r="H3" s="59"/>
+      <c r="I3" s="59" t="s">
         <v>163</v>
       </c>
-      <c r="J3" s="57"/>
-      <c r="K3" s="57" t="s">
+      <c r="J3" s="59"/>
+      <c r="K3" s="59" t="s">
         <v>171</v>
       </c>
-      <c r="L3" s="57"/>
-      <c r="M3" s="57" t="s">
+      <c r="L3" s="59"/>
+      <c r="M3" s="59" t="s">
         <v>137</v>
       </c>
-      <c r="N3" s="57"/>
-      <c r="P3" s="57" t="s">
+      <c r="N3" s="59"/>
+      <c r="P3" s="59" t="s">
         <v>139</v>
       </c>
-      <c r="Q3" s="57"/>
-      <c r="R3" s="57"/>
-      <c r="S3" s="57" t="s">
+      <c r="Q3" s="59"/>
+      <c r="R3" s="59"/>
+      <c r="S3" s="59" t="s">
         <v>163</v>
       </c>
-      <c r="T3" s="57"/>
-      <c r="U3" s="57" t="s">
+      <c r="T3" s="59"/>
+      <c r="U3" s="59" t="s">
         <v>137</v>
       </c>
-      <c r="V3" s="57"/>
-      <c r="W3" s="57" t="s">
+      <c r="V3" s="59"/>
+      <c r="W3" s="59" t="s">
         <v>171</v>
       </c>
-      <c r="X3" s="57"/>
+      <c r="X3" s="59"/>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B4" t="s">

</xml_diff>

<commit_message>
added AUC, KS, Gini and log-loss
</commit_message>
<xml_diff>
--- a/ACQ.Excel/Examples/ACQ.Options.xlsx
+++ b/ACQ.Excel/Examples/ACQ.Options.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\ACQ\ACQ.Excel\Examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B0010A3-C0B0-48A6-835C-6F4DAD829E24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{002EDA2F-B03A-47E9-B418-EFCF25818026}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1590" yWindow="1695" windowWidth="24450" windowHeight="12525" tabRatio="900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Utils" sheetId="3" r:id="rId1"/>
@@ -15977,7 +15977,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B2:N56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
@@ -16037,11 +16037,11 @@
       </c>
       <c r="H4" s="48">
         <f ca="1">TODAY()</f>
-        <v>44563</v>
+        <v>44564</v>
       </c>
       <c r="J4" s="49" t="str">
         <f ca="1">_xll.acq_tostring(H4)</f>
-        <v>44563</v>
+        <v>44564</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
@@ -16163,7 +16163,7 @@
       </c>
       <c r="H13" t="str">
         <f ca="1">_xll.acq_join(H3:H10)</f>
-        <v>3.14159265358979,44563,True,,,,,</v>
+        <v>3.14159265358979,44564,True,,,,,</v>
       </c>
     </row>
     <row r="14" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -16172,7 +16172,7 @@
       </c>
       <c r="H14" t="str">
         <f ca="1">_xll.acq_join(J3:J10, "|")</f>
-        <v>3.14159265358979|44563|TRUE|||||</v>
+        <v>3.14159265358979|44564|TRUE|||||</v>
       </c>
     </row>
     <row r="15" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -27090,7 +27090,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57EC0629-1DDD-4850-A456-ABCD64977042}">
   <dimension ref="B1:AK45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
@@ -51157,7 +51157,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BF3CA9D-20A9-4DB7-AD8A-F59DC22CC79A}">
   <dimension ref="A1:AA57"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B4" workbookViewId="0">
       <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>

</xml_diff>